<commit_message>
Made building models for furnace, archery target, coffin..
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="415">
   <si>
     <t>NONE</t>
   </si>
@@ -1252,6 +1252,18 @@
   </si>
   <si>
     <t>52:-1:-1</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Needs more coding</t>
   </si>
 </sst>
 </file>
@@ -2093,1219 +2105,1241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C206"/>
+  <dimension ref="B1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E1" t="s">
+        <v>412</v>
+      </c>
+      <c r="F1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="F7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>299</v>
@@ -3313,441 +3347,449 @@
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
+        <v>407</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
         <v>409</v>
       </c>
-      <c r="C206" s="1" t="s">
+      <c r="C207" s="1" t="s">
         <v>410</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made many more buildings. Todo: logic on the traps.
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="415">
   <si>
     <t>NONE</t>
   </si>
@@ -2107,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,6 +2200,9 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D8" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -2265,15 +2268,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>36</v>
       </c>
@@ -2297,7 +2303,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -2313,31 +2319,40 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>48</v>
       </c>
@@ -2345,7 +2360,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>50</v>
       </c>
@@ -2353,7 +2368,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>52</v>
       </c>
@@ -2361,7 +2376,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>54</v>
       </c>
@@ -2369,7 +2384,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>56</v>
       </c>
@@ -2377,7 +2392,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>58</v>
       </c>
@@ -2385,7 +2400,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>60</v>
       </c>
@@ -2649,7 +2664,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>126</v>
       </c>
@@ -2657,7 +2672,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>128</v>
       </c>
@@ -2665,7 +2680,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>130</v>
       </c>
@@ -2673,7 +2688,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>132</v>
       </c>
@@ -2681,7 +2696,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>134</v>
       </c>
@@ -2689,7 +2704,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>136</v>
       </c>
@@ -2697,7 +2712,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>138</v>
       </c>
@@ -2705,7 +2720,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>140</v>
       </c>
@@ -2713,7 +2728,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>142</v>
       </c>
@@ -2721,15 +2736,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>144</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>146</v>
       </c>
@@ -2737,7 +2755,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>148</v>
       </c>
@@ -2745,7 +2763,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>150</v>
       </c>
@@ -2753,7 +2771,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>152</v>
       </c>
@@ -2761,7 +2779,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>154</v>
       </c>
@@ -2769,7 +2787,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>156</v>
       </c>

</xml_diff>

<commit_message>
update building completion list.
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="415">
   <si>
     <t>NONE</t>
   </si>
@@ -2107,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2536,7 +2536,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>94</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>96</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>98</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>100</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>102</v>
       </c>
@@ -2576,15 +2576,18 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>104</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>106</v>
       </c>
@@ -2592,7 +2595,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>108</v>
       </c>
@@ -2600,7 +2603,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>110</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>112</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>114</v>
       </c>
@@ -2624,7 +2627,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>116</v>
       </c>
@@ -2632,7 +2635,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>118</v>
       </c>
@@ -2640,7 +2643,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>120</v>
       </c>
@@ -2648,7 +2651,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>122</v>
       </c>
@@ -2656,7 +2659,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>124</v>
       </c>
@@ -2679,6 +2682,9 @@
       <c r="C66" s="1" t="s">
         <v>129</v>
       </c>
+      <c r="D66" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
@@ -2686,6 +2692,9 @@
       </c>
       <c r="C67" s="1" t="s">
         <v>131</v>
+      </c>
+      <c r="D67" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made more small buildings.
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="415">
   <si>
     <t>NONE</t>
   </si>
@@ -2107,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="D193" sqref="D193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,6 +2189,9 @@
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D7" t="s">
+        <v>413</v>
+      </c>
       <c r="F7" t="s">
         <v>413</v>
       </c>
@@ -2359,6 +2362,9 @@
       <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="D26" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -2367,6 +2373,9 @@
       <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="D27" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -2594,6 +2603,9 @@
       <c r="C55" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="D55" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
@@ -3572,7 +3584,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>349</v>
       </c>
@@ -3580,7 +3592,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>351</v>
       </c>
@@ -3588,7 +3600,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>353</v>
       </c>
@@ -3596,7 +3608,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>355</v>
       </c>
@@ -3604,7 +3616,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>357</v>
       </c>
@@ -3612,7 +3624,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>359</v>
       </c>
@@ -3620,7 +3632,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>361</v>
       </c>
@@ -3628,7 +3640,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>363</v>
       </c>
@@ -3636,7 +3648,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>365</v>
       </c>
@@ -3644,7 +3656,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>367</v>
       </c>
@@ -3652,7 +3664,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>369</v>
       </c>
@@ -3660,7 +3672,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>371</v>
       </c>
@@ -3668,7 +3680,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>373</v>
       </c>
@@ -3676,7 +3688,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>375</v>
       </c>
@@ -3684,20 +3696,26 @@
         <v>376</v>
       </c>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>377</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D191" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>379</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>380</v>
+      </c>
+      <c r="D192" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added both forge types
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="415">
   <si>
     <t>Placeholder</t>
   </si>
@@ -1370,18 +1370,18 @@
   <dimension ref="B1:F207"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1712,6 +1712,9 @@
       <c r="C34" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="D34" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
@@ -1719,6 +1722,9 @@
       </c>
       <c r="C35" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added a bunch of workshop placeholders
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="415">
   <si>
     <t>Placeholder</t>
   </si>
@@ -1369,19 +1369,19 @@
   </sheetPr>
   <dimension ref="B1:F207"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,6 +1734,9 @@
       <c r="C36" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
@@ -1742,6 +1745,9 @@
       <c r="C37" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="D37" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
@@ -1750,6 +1756,9 @@
       <c r="C38" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="D38" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
@@ -1758,6 +1767,9 @@
       <c r="C39" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="D39" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
@@ -1766,6 +1778,9 @@
       <c r="C40" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="D40" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
@@ -1774,6 +1789,9 @@
       <c r="C41" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="D41" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
@@ -1782,6 +1800,9 @@
       <c r="C42" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="D42" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
@@ -1790,6 +1811,9 @@
       <c r="C43" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
@@ -1798,6 +1822,9 @@
       <c r="C44" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="D44" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
@@ -1806,6 +1833,9 @@
       <c r="C45" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="D45" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
@@ -1813,6 +1843,9 @@
       </c>
       <c r="C46" s="1" t="s">
         <v>93</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Finished placeholders for all non-custom workshops.
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="415">
   <si>
     <t>Placeholder</t>
   </si>
@@ -1369,19 +1369,16 @@
   </sheetPr>
   <dimension ref="B1:F207"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D49" activeCellId="0" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.280612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,6 +1852,9 @@
       <c r="C47" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="D47" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
@@ -1863,6 +1863,9 @@
       <c r="C48" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="D48" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
@@ -1871,6 +1874,9 @@
       <c r="C49" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="D49" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
@@ -1878,6 +1884,9 @@
       </c>
       <c r="C50" s="1" t="s">
         <v>101</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated building completion list.
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="978" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingList" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="421">
   <si>
     <t>Placeholder</t>
   </si>
@@ -1391,15 +1391,16 @@
   </sheetPr>
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.36224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8724489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,6 +2110,9 @@
       <c r="C61" s="0" t="s">
         <v>125</v>
       </c>
+      <c r="D61" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
@@ -2124,6 +2128,9 @@
       </c>
       <c r="C63" s="0" t="s">
         <v>129</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added nestbox, support, hive, bookcase buildings
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="421">
   <si>
     <t>Placeholder</t>
   </si>
@@ -1391,16 +1391,16 @@
   </sheetPr>
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D206" activeCellId="0" sqref="D206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,6 +2234,9 @@
       <c r="C75" s="0" t="s">
         <v>153</v>
       </c>
+      <c r="D75" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
@@ -3291,6 +3294,9 @@
       <c r="C206" s="0" t="s">
         <v>414</v>
       </c>
+      <c r="D206" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="0" t="s">
@@ -3314,6 +3320,9 @@
       </c>
       <c r="C209" s="0" t="s">
         <v>420</v>
+      </c>
+      <c r="D209" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enable instancing on building materials.
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="421">
   <si>
     <t>Placeholder</t>
   </si>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:F209"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D206" activeCellId="0" sqref="D206"/>
+      <selection pane="topLeft" activeCell="D205" activeCellId="0" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3270,6 +3270,9 @@
       <c r="C203" s="0" t="s">
         <v>408</v>
       </c>
+      <c r="D203" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="0" t="s">

</xml_diff>

<commit_message>
Added animated waterwheels and windmills
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="421">
   <si>
     <t>Placeholder</t>
   </si>
@@ -1392,15 +1392,15 @@
   <dimension ref="A1:F209"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D205" activeCellId="0" sqref="D205"/>
+      <selection pane="topLeft" activeCell="D200" activeCellId="0" sqref="D200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3246,6 +3246,9 @@
       <c r="C200" s="0" t="s">
         <v>402</v>
       </c>
+      <c r="D200" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="0" t="s">
@@ -3253,6 +3256,9 @@
       </c>
       <c r="C201" s="0" t="s">
         <v>404</v>
+      </c>
+      <c r="D201" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added an animated gear assembly.
</commit_message>
<xml_diff>
--- a/Assets/BuildingList.xlsx
+++ b/Assets/BuildingList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="421">
   <si>
     <t>Placeholder</t>
   </si>
@@ -1391,16 +1391,16 @@
   </sheetPr>
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D200" activeCellId="0" sqref="D200"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A183" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D197" activeCellId="0" sqref="D197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3221,6 +3221,9 @@
       </c>
       <c r="C197" s="0" t="s">
         <v>396</v>
+      </c>
+      <c r="D197" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>